<commit_message>
fix name error in code
</commit_message>
<xml_diff>
--- a/jiekoucase.xlsx
+++ b/jiekoucase.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wenge\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6695774-48E3-465D-AD92-9832C4B13AC2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="1770" yWindow="2880" windowWidth="23565" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,27 +22,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
-  <si>
-    <t>接口测试用例</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+  <si>
+    <t>接口</t>
   </si>
   <si>
     <t>编号</t>
   </si>
   <si>
-    <t>用例</t>
-  </si>
-  <si>
-    <t>项目</t>
-  </si>
-  <si>
-    <t>模块</t>
+    <t>项目名字</t>
+  </si>
+  <si>
+    <t>模块名字</t>
+  </si>
+  <si>
+    <t>接口名字</t>
   </si>
   <si>
     <t>接口url</t>
   </si>
   <si>
-    <t>请求协议</t>
+    <t>接口协议</t>
   </si>
   <si>
     <t>请求头</t>
@@ -45,69 +51,74 @@
     <t>请求方式</t>
   </si>
   <si>
-    <t>参数</t>
-  </si>
-  <si>
-    <t>断言</t>
-  </si>
-  <si>
-    <t>是否保存测试结果</t>
-  </si>
-  <si>
-    <t>是否依赖接口</t>
-  </si>
-  <si>
-    <t>依赖接口</t>
-  </si>
-  <si>
-    <t>依赖接口参数</t>
-  </si>
-  <si>
-    <t>是否查询数据库</t>
-  </si>
-  <si>
-    <t>数据库语句</t>
-  </si>
-  <si>
-    <t>数据库比较字段</t>
-  </si>
-  <si>
-    <t>昨夜西风凋碧树</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>http://www.tuling123.com/openapi/api</t>
+    <t>请求示例</t>
+  </si>
+  <si>
+    <t>请求返回示例</t>
+  </si>
+  <si>
+    <t>http</t>
   </si>
   <si>
     <t>asdfasdfadsf</t>
   </si>
   <si>
-    <t>POST</t>
-  </si>
-  <si>
-    <t>code=40007</t>
-  </si>
-  <si>
-    <t>的广东佛山高大上发个梵蒂冈</t>
-  </si>
-  <si>
-    <t>第三方割发代首法规的法规</t>
-  </si>
-  <si>
-    <t>的方式公司的分公司电饭锅</t>
-  </si>
-  <si>
-    <t>http</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>sddasdasdas</t>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>财务应付系统</t>
+  </si>
+  <si>
+    <t>应付数据线上化</t>
+  </si>
+  <si>
+    <t>应付数据线上化</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>应付数据线上化_ttl</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>应付数据线上化_ttk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>应付数据线上化_bbk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>应付数据线上化_bbc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://baike.baidu.com/api/openapi/BaikeLemmaCardApi?scope=103&amp;format=json&amp;appid=379020&amp;bk_key=%E9%93%B6%E9%AD%82&amp;bk_length=600</t>
+  </si>
+  <si>
+    <t>http://baike.baidu.com/api/openapi/BaikeLemmaCardApi?scope=103&amp;format=json&amp;appid=379020&amp;bk_key=&amp;bk_length=600</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://baike.baidu.com/api/openapi/BaikeLemmaCardApi?scope=103&amp;format=json&amp;appid=379020&amp;bk_key=%E9%93%B6%E9%AD%82&amp;bk_length=600</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://baike.baidu.com/api/openapi/BaikeLemmaCardApi?scope=103&amp;format=json&amp;appid=379020&amp;bk_key=银魂&amp;bk_length=600</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +127,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -139,36 +173,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -460,260 +504,234 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="9" style="2"/>
-    <col min="3" max="6" width="9" style="1"/>
-    <col min="7" max="7" width="14.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9" style="1"/>
-    <col min="9" max="9" width="18.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.25" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="12.375" customWidth="1"/>
+    <col min="2" max="2" width="13.625" customWidth="1"/>
+    <col min="3" max="3" width="14.75" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="74.25" customWidth="1"/>
+    <col min="7" max="7" width="30.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
         <v>13</v>
       </c>
-      <c r="N2" t="s">
+      <c r="J3" t="s">
         <v>14</v>
       </c>
-      <c r="O2" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" t="s">
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="1" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>27</v>
+      <c r="F6" t="s">
+        <v>11</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="C9" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B1:J1"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{DA124362-6EE2-4878-A032-6B8ACAA39781}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{D70305D3-7A10-439A-A8AA-1BB3C59D2F9A}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{C59BDC7C-D600-4271-9483-710D944C2A8A}"/>
+  </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>